<commit_message>
Dodani afrikati, exportovani .pdf file-ovi
</commit_message>
<xml_diff>
--- a/Bolnica/Use case scenarij/Apoteka.xlsx
+++ b/Bolnica/Use case scenarij/Apoteka.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t xml:space="preserve">Scenarij </t>
   </si>
@@ -38,9 +38,6 @@
     <t>Opis:</t>
   </si>
   <si>
-    <t xml:space="preserve">Pacijent podize lijekove </t>
-  </si>
-  <si>
     <t>Preduvjeti:</t>
   </si>
   <si>
@@ -77,15 +74,6 @@
     <t>3.Predaje zahtjev za preuzimanje lijeka</t>
   </si>
   <si>
-    <t>10.Oznacava da su lijekovi podignuti</t>
-  </si>
-  <si>
-    <t>11.Salje izvjestaj osiguravajucoj kuci</t>
-  </si>
-  <si>
-    <t>Baza podataka/sistem</t>
-  </si>
-  <si>
     <t>Lijekovi nisu na stanju</t>
   </si>
   <si>
@@ -98,15 +86,9 @@
     <t>1.Odabrani lijekovi nisu na stanju</t>
   </si>
   <si>
-    <t>2.Salje zahtjev za nabavku lijekova</t>
-  </si>
-  <si>
     <t>Alternativni tok:</t>
   </si>
   <si>
-    <t>Zahtjev za preuzimanje lijeka neuspjesan</t>
-  </si>
-  <si>
     <t>Preduvjet:</t>
   </si>
   <si>
@@ -131,9 +113,6 @@
     <t>Alternativni tok 2.</t>
   </si>
   <si>
-    <t>Identifikacija pacijenta neuspjesna</t>
-  </si>
-  <si>
     <t>1.Daje informaciju da identifikacija pacijenta nije uspjela</t>
   </si>
   <si>
@@ -179,13 +158,31 @@
     <t xml:space="preserve">Alternativni tok 4. </t>
   </si>
   <si>
-    <t>Na koraku 8. glavnog toka, utvrdjeno da lijekovi nisu na stanju</t>
-  </si>
-  <si>
     <t>Pacijent preuzima lijek, lijek se dodaje u listu za nabavku</t>
   </si>
   <si>
     <t>3.Dodaje lijekove u listu za nabavku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pacijent podiže lijekove </t>
+  </si>
+  <si>
+    <t>Zahtjev za preuzimanje lijeka neuspješan</t>
+  </si>
+  <si>
+    <t>10.Označava da su lijekovi podignuti</t>
+  </si>
+  <si>
+    <t>11.Šalje izvještaj osiguravajućoj kući</t>
+  </si>
+  <si>
+    <t>Identifikacija pacijenta neuspješna</t>
+  </si>
+  <si>
+    <t>Na koraku 8. glavnog toka, utvrđeno da lijekovi nisu na stanju</t>
+  </si>
+  <si>
+    <t>2.Šalje zahtjev za nabavku lijekova</t>
   </si>
 </sst>
 </file>
@@ -254,12 +251,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -268,6 +259,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,160 +596,160 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
+      <c r="B3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="7"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
-        <v>38</v>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
-        <v>39</v>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
-        <v>42</v>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
-        <v>18</v>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,21 +764,21 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -789,29 +786,29 @@
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>22</v>
+      <c r="A29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
-        <v>32</v>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="6"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
@@ -825,21 +822,21 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
@@ -847,57 +844,57 @@
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>22</v>
+      <c r="A37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6" t="s">
-        <v>36</v>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="6"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -905,107 +902,107 @@
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>22</v>
+      <c r="A45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6" t="s">
-        <v>48</v>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="6"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="4"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>22</v>
+      <c r="A54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8" t="s">
-        <v>23</v>
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56" s="8"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="6"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8" t="s">
-        <v>53</v>
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>